<commit_message>
brand crawling 공백 제거
</commit_message>
<xml_diff>
--- a/celeb/actor_cinema_2023.xlsx
+++ b/celeb/actor_cinema_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimkyuri/Documents/학교공부/4-1/sluv/crawling/celeb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A94710A-99D8-7940-9FA8-CA3852DB2EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31270EF1-50C1-9948-B24E-B9E9B6C76083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4115,7 +4115,7 @@
   <dimension ref="A1:D625"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H7" sqref="H6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>

</xml_diff>